<commit_message>
Update with today's bets
</commit_message>
<xml_diff>
--- a/Bets.xlsx
+++ b/Bets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Desktop\github\nba_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90FB5B5-3E14-4950-91C5-7DE1A13E6E0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2108AD-0E15-4AC7-91CA-A172EAD33E3A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="2" xr2:uid="{2A9291FE-3680-40F6-A028-104B01FB4D86}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{2A9291FE-3680-40F6-A028-104B01FB4D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
   <si>
     <t>Market</t>
   </si>
@@ -135,6 +135,78 @@
   </si>
   <si>
     <t>Cumulative Net Profit</t>
+  </si>
+  <si>
+    <t>Juan Hernangomez under 11.5</t>
+  </si>
+  <si>
+    <t>Deandre Ayton over 16.5</t>
+  </si>
+  <si>
+    <t>Pascal Siakam under 17.5</t>
+  </si>
+  <si>
+    <t>Fred VanVleet under 14.5</t>
+  </si>
+  <si>
+    <t>Trevor Ariza Under (13.5)</t>
+  </si>
+  <si>
+    <t>Joel Embiid Under (25.5)</t>
+  </si>
+  <si>
+    <t>Dwyane Wade Under (13.5)</t>
+  </si>
+  <si>
+    <t>Brook Lopez Under (4.5 REB)</t>
+  </si>
+  <si>
+    <t>Giannis Antetokounmpo Under (6.5 AST)</t>
+  </si>
+  <si>
+    <t>James Harden Under (33.5)</t>
+  </si>
+  <si>
+    <t>Eric Gordon Under (18.5)</t>
+  </si>
+  <si>
+    <t>Clint Capela Under (15.5)</t>
+  </si>
+  <si>
+    <t>PJ Tucker Under (9.5)</t>
+  </si>
+  <si>
+    <t>James Harden Under (6.5 rebounds)</t>
+  </si>
+  <si>
+    <t>Houston Win</t>
+  </si>
+  <si>
+    <t>Juancho Hernangomez Under (12.5)</t>
+  </si>
+  <si>
+    <t>Lou Williams Over (16.5)</t>
+  </si>
+  <si>
+    <t>Denver win</t>
+  </si>
+  <si>
+    <t>Stephen Curry Under (28.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Durant Over (5.5 AST) </t>
+  </si>
+  <si>
+    <t>Luka Doncic under 5.5 AST</t>
+  </si>
+  <si>
+    <t>lose</t>
+  </si>
+  <si>
+    <t>Wizards win</t>
+  </si>
+  <si>
+    <t>Checked</t>
   </si>
 </sst>
 </file>
@@ -144,7 +216,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-C09]* #,##0.00_-;\-[$$-C09]* #,##0.00_-;_-[$$-C09]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -295,9 +367,8 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -341,9 +412,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -370,7 +438,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -396,13 +464,163 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -421,6 +639,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6969"/>
       <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
@@ -495,6 +714,9 @@
                 <c:pt idx="2">
                   <c:v>43456</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43457</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -512,6 +734,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,6 +789,9 @@
                 <c:pt idx="2">
                   <c:v>43456</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43457</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -577,10 +805,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.457499999999996</c:v>
+                  <c:v>40.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.1000000000000085</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,10 +874,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.457499999999996</c:v>
+                  <c:v>40.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.557500000000005</c:v>
+                  <c:v>45.560000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -830,6 +1064,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="746731440"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1815,42 +2050,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="36">
+      <c r="B3" s="34">
         <f>COUNTA(Master!A:A)-1</f>
-        <v>11</v>
-      </c>
-      <c r="C3" s="23">
+        <v>33</v>
+      </c>
+      <c r="C3" s="21">
         <f>SUM(Master!E:E)</f>
-        <v>105</v>
-      </c>
-      <c r="D3" s="23">
+        <v>237</v>
+      </c>
+      <c r="D3" s="21">
         <f>SUM(Master!G:G)</f>
-        <v>46.000000000000007</v>
-      </c>
-      <c r="E3" s="23">
+        <v>82.200000000000017</v>
+      </c>
+      <c r="E3" s="21">
         <f>SUM(Master!J:J)</f>
-        <v>45.557500000000005</v>
-      </c>
-      <c r="F3" s="37">
+        <v>81.250000000000014</v>
+      </c>
+      <c r="F3" s="35">
         <f>E3/C3</f>
-        <v>0.43388095238095242</v>
+        <v>0.34282700421940937</v>
       </c>
     </row>
   </sheetData>
@@ -1862,145 +2097,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A4DC74-5C2D-4463-A37B-252BAD15DE0C}">
   <dimension ref="B2:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.21875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="16" customWidth="1"/>
-    <col min="4" max="7" width="16.21875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="15" customWidth="1"/>
+    <col min="4" max="7" width="16.21875" style="17" customWidth="1"/>
     <col min="8" max="8" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="33">
+      <c r="B3" s="31">
         <v>43452</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <f>COUNTIF(Master!A:A,'Day by Day'!B3)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="27">
         <f>SUMIFS(Master!E:E,Master!A:A, 'Day by Day'!B3)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="27">
         <f>SUMIFS(Master!G:G,Master!A:A,'Day by Day'!B3)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="27">
         <f>SUMIFS(Master!I:I,Master!A:A,'Day by Day'!B3)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="27">
         <f>SUMIFS(Master!J:J,Master!A:A,'Day by Day'!B3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="28">
         <f>IFERROR(G3/D3,0)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="29">
         <f>SUM($G$3:G3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>43453</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <f>COUNTIF(Master!A:A,'Day by Day'!B4)</f>
         <v>5</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <f>SUMIFS(Master!E:E,Master!A:A, 'Day by Day'!B4)</f>
         <v>35</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>SUMIFS(Master!G:G,Master!A:A,'Day by Day'!B4)</f>
         <v>40.9</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <f>SUMIFS(Master!I:I,Master!A:A,'Day by Day'!B4)</f>
-        <v>-0.44250000000000012</v>
-      </c>
-      <c r="G4" s="18">
+        <v>-0.44</v>
+      </c>
+      <c r="G4" s="17">
         <f>SUMIFS(Master!J:J,Master!A:A,'Day by Day'!B4)</f>
-        <v>40.457499999999996</v>
-      </c>
-      <c r="H4" s="14">
+        <v>40.46</v>
+      </c>
+      <c r="H4" s="13">
         <f t="shared" ref="H4:H5" si="0">IFERROR(G4/D4,0)</f>
-        <v>1.1559285714285714</v>
-      </c>
-      <c r="I4" s="15">
+        <v>1.1559999999999999</v>
+      </c>
+      <c r="I4" s="14">
         <f>SUM($G$3:G4)</f>
-        <v>40.457499999999996</v>
+        <v>40.46</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>43456</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <f>COUNTIF(Master!A:A,'Day by Day'!B5)</f>
         <v>6</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f>SUMIFS(Master!E:E,Master!A:A, 'Day by Day'!B5)</f>
         <v>70</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>SUMIFS(Master!G:G,Master!A:A,'Day by Day'!B5)</f>
         <v>5.1000000000000085</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <f>SUMIFS(Master!I:I,Master!A:A,'Day by Day'!B5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <f>SUMIFS(Master!J:J,Master!A:A,'Day by Day'!B5)</f>
         <v>5.1000000000000085</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <f t="shared" si="0"/>
         <v>7.2857142857142981E-2</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <f>SUM($G$3:G5)</f>
-        <v>45.557500000000005</v>
+        <v>45.560000000000009</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I6" s="15"/>
+      <c r="B6" s="16">
+        <v>43457</v>
+      </c>
+      <c r="C6" s="15">
+        <f>COUNTIF(Master!A:A,'Day by Day'!B6)</f>
+        <v>22</v>
+      </c>
+      <c r="D6" s="17">
+        <f>SUMIFS(Master!E:E,Master!A:A, 'Day by Day'!B6)</f>
+        <v>132</v>
+      </c>
+      <c r="E6" s="17">
+        <f>SUMIFS(Master!G:G,Master!A:A,'Day by Day'!B6)</f>
+        <v>36.199999999999996</v>
+      </c>
+      <c r="F6" s="17">
+        <f>SUMIFS(Master!I:I,Master!A:A,'Day by Day'!B6)</f>
+        <v>-0.51</v>
+      </c>
+      <c r="G6" s="17">
+        <f>SUMIFS(Master!J:J,Master!A:A,'Day by Day'!B6)</f>
+        <v>35.69</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ref="H6" si="1">IFERROR(G6/D6,0)</f>
+        <v>0.27037878787878789</v>
+      </c>
+      <c r="I6" s="14">
+        <f>SUM($G$3:G6)</f>
+        <v>81.25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2011,61 +2276,65 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C5EB38-0E05-412E-AA6C-435877CED8A2}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="38" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="36" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="6"/>
-    <col min="5" max="5" width="8.88671875" style="8"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="15"/>
+    <col min="4" max="4" width="8.88671875" style="5"/>
+    <col min="5" max="5" width="8.88671875" style="7"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="38">
+      <c r="K2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="36">
         <v>43453</v>
       </c>
       <c r="B3" t="s">
@@ -2074,30 +2343,33 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>8.4</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G4" si="0">IF(F3="", 0, IF(F3="Win", E3*D3-E3, -E3))</f>
         <v>37</v>
       </c>
-      <c r="I3" s="15">
-        <f t="shared" ref="I3:I13" si="1">-H3*G3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I26" si="1">ROUND(-H3*G3, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="14">
         <f t="shared" ref="J3:J13" si="2">G3+I3</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="38">
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="36">
         <v>43453</v>
       </c>
       <c r="B4" t="s">
@@ -2106,30 +2378,33 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
         <v>5.0499999999999989</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="14">
         <f t="shared" si="2"/>
         <v>5.0499999999999989</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="38">
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="36">
         <v>43453</v>
       </c>
       <c r="B5" t="s">
@@ -2138,30 +2413,33 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1.85</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G13" si="3">IF(F5="", 0, IF(F5="Win", E5*D5-E5, -E5))</f>
         <v>-5</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="14">
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="38">
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="36">
         <v>43453</v>
       </c>
       <c r="B6" t="s">
@@ -2170,30 +2448,33 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>1.87</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
         <v>-5</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="14">
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="38">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="36">
         <v>43453</v>
       </c>
       <c r="B7" t="s">
@@ -2202,65 +2483,72 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>1.59</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>15</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
         <v>8.8500000000000014</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="47">
         <v>0.05</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <f t="shared" si="1"/>
-        <v>-0.44250000000000012</v>
-      </c>
-      <c r="J7" s="23">
+        <v>-0.44</v>
+      </c>
+      <c r="J7" s="21">
         <f t="shared" si="2"/>
-        <v>8.4075000000000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40">
+        <v>8.4100000000000019</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
         <v>43456</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>3.15</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>10</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <f t="shared" si="3"/>
         <v>-10</v>
       </c>
-      <c r="I8" s="26">
+      <c r="H8" s="4"/>
+      <c r="I8" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="38">
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="36">
         <v>43456</v>
       </c>
       <c r="B9" t="s">
@@ -2269,30 +2557,33 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1.87</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>20</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
         <v>17.400000000000006</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <f t="shared" si="2"/>
         <v>17.400000000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="38">
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="36">
         <v>43456</v>
       </c>
       <c r="B10" t="s">
@@ -2301,30 +2592,33 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>1.87</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>10</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
         <v>8.7000000000000028</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <f t="shared" si="2"/>
         <v>8.7000000000000028</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="36">
         <v>43456</v>
       </c>
       <c r="B11" t="s">
@@ -2333,30 +2627,33 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>1.8</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
         <v>-10</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="14">
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="38">
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="36">
         <v>43456</v>
       </c>
       <c r="B12" t="s">
@@ -2365,70 +2662,861 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>1.9</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>10</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="22">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
         <v>43456</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="40">
         <v>2.02</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="41">
         <v>10</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f t="shared" si="3"/>
         <v>-10</v>
       </c>
-      <c r="I13" s="23">
+      <c r="H13" s="42"/>
+      <c r="I13" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="45">
+      <c r="J13" s="43">
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="21"/>
+      <c r="K13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.95</v>
+      </c>
+      <c r="E14" s="7">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G29" si="4">IF(F14="", 0, IF(F14="Win", E14*D14-E14, -E14))</f>
+        <v>4.75</v>
+      </c>
+      <c r="I14" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" ref="J14:J29" si="5">G14+I14</f>
+        <v>4.75</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="E15" s="7">
+        <v>10</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>-10</v>
+      </c>
+      <c r="I15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="14">
+        <f t="shared" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="E16" s="7">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>8.7000000000000028</v>
+      </c>
+      <c r="I16" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="5"/>
+        <v>8.7000000000000028</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.93</v>
+      </c>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+      <c r="I17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="E18" s="7">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+      <c r="I18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1.79</v>
+      </c>
+      <c r="E19" s="7">
+        <v>5</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>3.9499999999999993</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="5"/>
+        <v>3.9499999999999993</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2.14</v>
+      </c>
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>5.7000000000000011</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" si="5"/>
+        <v>5.7000000000000011</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.78</v>
+      </c>
+      <c r="E21" s="7">
+        <v>5</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="5"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.82</v>
+      </c>
+      <c r="E22" s="7">
+        <v>5</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1.86</v>
+      </c>
+      <c r="E23" s="7">
+        <v>5</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>4.3000000000000007</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="14">
+        <f t="shared" si="5"/>
+        <v>4.3000000000000007</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1.94</v>
+      </c>
+      <c r="E24" s="7">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="14">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2.02</v>
+      </c>
+      <c r="E25" s="7">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
+        <f t="shared" si="5"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1.74</v>
+      </c>
+      <c r="E26" s="7">
+        <v>5</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>3.6999999999999993</v>
+      </c>
+      <c r="I26" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="14">
+        <f t="shared" si="5"/>
+        <v>3.6999999999999993</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1.52</v>
+      </c>
+      <c r="E27" s="7">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="H27" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="I27" s="14">
+        <f>ROUND(-H27*G27, 2)</f>
+        <v>-0.26</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" si="5"/>
+        <v>4.9399999999999995</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1.74</v>
+      </c>
+      <c r="E28" s="7">
+        <v>5</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>3.6999999999999993</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" ref="I28:I35" si="6">ROUND(-H28*G28, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="14">
+        <f t="shared" si="5"/>
+        <v>3.6999999999999993</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1.79</v>
+      </c>
+      <c r="E29" s="7">
+        <v>5</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="14">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1.91</v>
+      </c>
+      <c r="E30" s="7">
+        <v>5</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G31" si="7">IF(F30="", 0, IF(F30="Win", E30*D30-E30, -E30))</f>
+        <v>4.5499999999999989</v>
+      </c>
+      <c r="I30" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
+        <f t="shared" ref="J30:J31" si="8">G30+I30</f>
+        <v>4.5499999999999989</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E31" s="7">
+        <v>5</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="I31" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="14">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="E32" s="7">
+        <v>5</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ref="G32:G35" si="9">IF(F32="", 0, IF(F32="Win", E32*D32-E32, -E32))</f>
+        <v>4.3500000000000014</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="14">
+        <f t="shared" ref="J32:J35" si="10">G32+I32</f>
+        <v>4.3500000000000014</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E33" s="7">
+        <v>5</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="9"/>
+        <v>5.35</v>
+      </c>
+      <c r="I33" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="14">
+        <f t="shared" si="10"/>
+        <v>5.35</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2.15</v>
+      </c>
+      <c r="E34" s="7">
+        <v>7</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>8.0499999999999989</v>
+      </c>
+      <c r="I34" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="14">
+        <f t="shared" si="10"/>
+        <v>8.0499999999999989</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="36">
+        <v>43457</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1.49</v>
+      </c>
+      <c r="E35" s="7">
+        <v>10</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H35" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="I35" s="14">
+        <f t="shared" si="6"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J35" s="14">
+        <f t="shared" si="10"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>AND(F3&lt;&gt;"Win", F3&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>F3="Win"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Betfair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Sportsbet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Ladbrokes"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update bets and change asthetics of arbe and cross tabs
</commit_message>
<xml_diff>
--- a/Bets.xlsx
+++ b/Bets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Desktop\github\nba_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCFBCF5-ACBC-4AEB-9913-42012620BA50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94B0E05-4D70-40A3-8EDC-A0C84C14E735}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{2A9291FE-3680-40F6-A028-104B01FB4D86}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="2" xr2:uid="{2A9291FE-3680-40F6-A028-104B01FB4D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="3" r:id="rId1"/>
@@ -22,11 +22,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Master!$A$2:$N$118</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'Day by Day'!$B$19:$B$32</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Day by Day'!$B$19:$B$33</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Day by Day'!$H$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Day by Day'!$H$19:$H$32</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Day by Day'!$H$19:$H$33</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Day by Day'!$B$19:$B$34</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Day by Day'!$H$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Day by Day'!$H$19:$H$34</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">Cross!$C$6,Cross!$E$6</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
@@ -43,7 +41,7 @@
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">Cross!$E$10</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Cross!$C$14</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
@@ -57,7 +55,7 @@
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
@@ -77,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="244">
   <si>
     <t>Market</t>
   </si>
@@ -496,9 +494,6 @@
     <t>x wins</t>
   </si>
   <si>
-    <t>Profit</t>
-  </si>
-  <si>
     <t>y wins</t>
   </si>
   <si>
@@ -562,9 +557,6 @@
     <t>Under</t>
   </si>
   <si>
-    <t>Pr</t>
-  </si>
-  <si>
     <t>Over and under</t>
   </si>
   <si>
@@ -791,17 +783,42 @@
   </si>
   <si>
     <t>Danilo Gallinari under 6.5 REB</t>
+  </si>
+  <si>
+    <t>Russell Westbrook under 12.5 AST</t>
+  </si>
+  <si>
+    <t>Jerami Grant under 5.5 REB</t>
+  </si>
+  <si>
+    <t>Kyle Kuzma under 3.5 AST</t>
+  </si>
+  <si>
+    <t>Profit:</t>
+  </si>
+  <si>
+    <t>Pr over</t>
+  </si>
+  <si>
+    <t>Pr under</t>
+  </si>
+  <si>
+    <t>Worst case</t>
+  </si>
+  <si>
+    <t>Best case</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-C09]* #,##0.00_-;\-[$$-C09]* #,##0.00_-;_-[$$-C09]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -853,15 +870,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1012,13 +1035,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1198,10 +1247,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1432,6 +1554,9 @@
                 <c:pt idx="14">
                   <c:v>43480</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>43481</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1485,6 +1610,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1572,6 +1700,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>43480</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1725,6 +1856,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>74.84999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>104.64999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,10 +2091,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1970,7 +2104,7 @@
         <cx:series layoutId="waterfall" uniqueId="{A02B1098-E631-4E5D-8703-8B01B02E2E08}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v> Net profit </cx:v>
             </cx:txData>
           </cx:tx>
@@ -3505,7 +3639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AE740B-DE5B-4DA0-BB8C-CF8C70395C12}">
   <dimension ref="B2:K3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -3548,34 +3682,34 @@
         <v>79</v>
       </c>
       <c r="J2" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K2" s="90"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
         <f>COUNTA(Master!A:A)-1</f>
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C3" s="20">
         <f>SUM(Master!F:F)</f>
-        <v>2993.92</v>
+        <v>3023.92</v>
       </c>
       <c r="D3" s="20">
         <f>SUM(Master!J:J)</f>
-        <v>82.230000000000047</v>
+        <v>112.03000000000004</v>
       </c>
       <c r="E3" s="20">
         <f>SUM(Master!M:M)</f>
-        <v>74.850000000000065</v>
+        <v>104.65000000000006</v>
       </c>
       <c r="F3" s="33">
         <f>E3/C3</f>
-        <v>2.5000668020521612E-2</v>
+        <v>3.4607397021085236E-2</v>
       </c>
       <c r="G3" s="51">
         <f>COUNTIF(Master!$I:$I, G2)</f>
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H3" s="2">
         <f>COUNTIF(Master!$I:$I, H2)</f>
@@ -3583,11 +3717,11 @@
       </c>
       <c r="I3" s="33">
         <f>G3/SUM(G3:H3)</f>
-        <v>0.55660377358490565</v>
+        <v>0.56279069767441858</v>
       </c>
       <c r="J3" s="92">
         <f>SUMPRODUCT(Master!F:F, Master!D:D)/SUM(Master!F:F)</f>
-        <v>1.9488396483539967</v>
+        <v>1.9492810656366566</v>
       </c>
     </row>
   </sheetData>
@@ -3597,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A4DC74-5C2D-4463-A37B-252BAD15DE0C}">
-  <dimension ref="B18:K33"/>
+  <dimension ref="B18:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3645,7 +3779,7 @@
         <v>32</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
@@ -3684,10 +3818,7 @@
         <f>SUM($H$19:H19)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="12" t="e">
-        <f>COUNTIFS(Master!A:A, 'Day by Day'!B19, Master!I:I, "Win")/COUNTIFS(Master!A:A, 'Day by Day'!B19)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="15">
@@ -4261,6 +4392,47 @@
       <c r="K33" s="12">
         <f>COUNTIFS(Master!A:A, 'Day by Day'!B33, Master!I:I, "Win")/COUNTIFS(Master!A:A, 'Day by Day'!B33)</f>
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="15">
+        <v>43481</v>
+      </c>
+      <c r="C34" s="14">
+        <f>COUNTIF(Master!A:A,'Day by Day'!B34)</f>
+        <v>3</v>
+      </c>
+      <c r="D34" s="16">
+        <f>SUMIFS(Master!F:F,Master!A:A, 'Day by Day'!B34)</f>
+        <v>30</v>
+      </c>
+      <c r="E34" s="16">
+        <f>SUMIFS(Master!H:H,Master!A:A,'Day by Day'!B34)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <f>SUMIFS(Master!J:J,Master!A:A,'Day by Day'!B34)</f>
+        <v>29.8</v>
+      </c>
+      <c r="G34" s="16">
+        <f>SUMIFS(Master!L:L,Master!A:A,'Day by Day'!B34)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="16">
+        <f>SUMIFS(Master!M:M,Master!A:A,'Day by Day'!B34)</f>
+        <v>29.8</v>
+      </c>
+      <c r="I34" s="12">
+        <f t="shared" ref="I34" si="13">IFERROR(H34/D34,0)</f>
+        <v>0.9933333333333334</v>
+      </c>
+      <c r="J34" s="13">
+        <f>SUM($H$19:H34)</f>
+        <v>104.64999999999998</v>
+      </c>
+      <c r="K34" s="12">
+        <f>COUNTIFS(Master!A:A, 'Day by Day'!B34, Master!I:I, "Win")/COUNTIFS(Master!A:A, 'Day by Day'!B34)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4272,166 +4444,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD5CC70-3B01-4547-8649-2574819AA279}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="121">
+        <v>14.5</v>
+      </c>
+      <c r="D2" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="C2">
-        <v>14.5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2">
+      <c r="E2" s="122">
         <v>15.5</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="123">
         <v>1.87</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="124">
         <v>1.71</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="123">
         <v>2.33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="124">
         <v>1.46</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="100" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="125">
         <f>1/C4</f>
         <v>0.42918454935622319</v>
       </c>
-      <c r="D5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="119" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="126">
         <f>1/E4</f>
         <v>0.68493150684931503</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
+      <c r="C6" s="127">
+        <v>48</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="128">
+        <v>52</v>
+      </c>
+      <c r="F6" s="129">
         <f>E6+C6</f>
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E8" s="94" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="69" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9">
+      <c r="C9" s="118">
         <f>1-E5</f>
         <v>0.31506849315068497</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="22">
         <f>C6*C3-F6</f>
-        <v>7.4000000000000057</v>
-      </c>
-      <c r="E9">
+        <v>-10.239999999999995</v>
+      </c>
+      <c r="E9" s="66">
         <f>C9*D9</f>
-        <v>2.3315068493150704</v>
+        <v>-3.2263013698630125</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="119">
         <f>1-C5</f>
         <v>0.57081545064377681</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="45">
         <f>E6*E3-F6</f>
-        <v>-12.899999999999999</v>
-      </c>
-      <c r="E10">
+        <v>-11.079999999999998</v>
+      </c>
+      <c r="E10" s="46">
         <f t="shared" ref="E10:E11" si="0">C10*D10</f>
-        <v>-7.3635193133047201</v>
+        <v>-6.3246351931330462</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="93">
+      <c r="B11" s="101" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="120">
         <f>1-SUM(C9:C10)</f>
         <v>0.11411605620553822</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="20">
         <f>C6*C3+E6*E3-F6</f>
-        <v>24.500000000000007</v>
-      </c>
-      <c r="E11">
+        <v>78.680000000000007</v>
+      </c>
+      <c r="E11" s="72">
         <f t="shared" si="0"/>
-        <v>2.7958433770356872</v>
+        <v>8.9786513022517482</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="B12" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="117">
         <f>SUM(C9:C11)</f>
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="2"/>
+      <c r="E12" s="72">
         <f>SUM(E9:E11)</f>
-        <v>-2.236169086953963</v>
+        <v>-0.57228526074431052</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" s="13">
+        <f>MIN(D9:D11)</f>
+        <v>-11.079999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C15" s="13">
+        <f>MAX(D9:D11)</f>
+        <v>78.680000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -4441,141 +4634,144 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAA8682-750D-4886-9CF0-12B295781815}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B2:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+      <c r="B2" s="77"/>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="99" t="s">
         <v>135</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="110" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="J2" s="106" t="s">
         <v>138</v>
       </c>
-      <c r="K2" t="s">
-        <v>140</v>
+      <c r="K2" s="107" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="98">
         <v>2.25</v>
       </c>
-      <c r="D3">
-        <f>IF(D6, 1, "")</f>
+      <c r="D3" s="115">
+        <f>IF(C5, 1, "")</f>
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="111">
         <f>D3*C3-D3</f>
         <v>1.25</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="112">
         <f>-D3</f>
         <v>-1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="102">
         <v>24</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="96">
         <f>ROUND(D3,2)</f>
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="70">
         <f>H3*C3-H3</f>
         <v>30</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="108">
         <f>-H3</f>
         <v>-24</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="100" t="s">
         <v>137</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="95">
         <v>1.87</v>
       </c>
-      <c r="D4">
-        <f>IF(D6, C3/C4, "")</f>
+      <c r="D4" s="116">
+        <f>IF(C5, C3/C4, "")</f>
         <v>1.2032085561497325</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="113">
         <f>-D4</f>
         <v>-1.2032085561497325</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="114">
         <f>D4*C4-D4</f>
         <v>1.0467914438502675</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="97">
         <v>28</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <f>ROUND(D4,2)</f>
         <v>1.2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="39">
         <f>-H4</f>
         <v>-28</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="109">
         <f>H4*C4-H4</f>
         <v>24.36</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5">
+      <c r="B5" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="104" t="b">
+        <f>1/C3+1/C4 &lt; 1</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" s="113">
         <f>SUM(E3:E4)</f>
         <v>4.6791443850267456E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="114">
         <f>SUM(F3:F4)</f>
         <v>4.6791443850267456E-2</v>
       </c>
-      <c r="J5">
+      <c r="I5" s="105" t="s">
+        <v>239</v>
+      </c>
+      <c r="J5" s="106">
         <f>SUM(J3:J4)</f>
         <v>2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="107">
         <f>SUM(K3:K4)</f>
         <v>0.35999999999999943</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" t="b">
-        <f>1/C3+1/C4 &lt; 1</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4585,11 +4781,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C5EB38-0E05-412E-AA6C-435877CED8A2}">
-  <dimension ref="A1:Q214"/>
+  <dimension ref="A1:Q217"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M206" sqref="M206:M210"/>
+      <pane ySplit="2" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I218" sqref="I218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8977,7 +9173,7 @@
         <v>9</v>
       </c>
       <c r="C109" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D109" s="5">
         <v>2.0699999999999998</v>
@@ -9023,7 +9219,7 @@
         <v>9</v>
       </c>
       <c r="C110" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D110" s="5">
         <v>1.8</v>
@@ -9069,7 +9265,7 @@
         <v>9</v>
       </c>
       <c r="C111" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D111" s="5">
         <v>1.95</v>
@@ -9115,7 +9311,7 @@
         <v>9</v>
       </c>
       <c r="C112" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D112" s="5">
         <v>1.91</v>
@@ -9161,7 +9357,7 @@
         <v>10</v>
       </c>
       <c r="C113" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D113" s="5">
         <v>2.1</v>
@@ -9207,7 +9403,7 @@
         <v>10</v>
       </c>
       <c r="C114" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D114" s="5">
         <v>2.1</v>
@@ -9253,7 +9449,7 @@
         <v>9</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D115" s="5">
         <v>1.61</v>
@@ -9299,7 +9495,7 @@
         <v>10</v>
       </c>
       <c r="C116" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D116" s="5">
         <v>2.0499999999999998</v>
@@ -9345,7 +9541,7 @@
         <v>9</v>
       </c>
       <c r="C117" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D117" s="5">
         <v>2.09</v>
@@ -9391,7 +9587,7 @@
         <v>9</v>
       </c>
       <c r="C118" s="83" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D118" s="56">
         <v>1.75</v>
@@ -9435,7 +9631,7 @@
         <v>9</v>
       </c>
       <c r="C119" s="40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D119" s="5">
         <v>1.77</v>
@@ -9467,7 +9663,7 @@
         <v>5</v>
       </c>
       <c r="C120" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D120" s="5">
         <v>1</v>
@@ -9499,7 +9695,7 @@
         <v>5</v>
       </c>
       <c r="C121" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D121" s="5">
         <v>2</v>
@@ -9569,7 +9765,7 @@
         <v>10</v>
       </c>
       <c r="C123" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D123" s="5">
         <v>2</v>
@@ -9601,7 +9797,7 @@
         <v>10</v>
       </c>
       <c r="C124" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D124" s="5">
         <v>1.91</v>
@@ -9633,7 +9829,7 @@
         <v>9</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D125" s="7">
         <v>2.06</v>
@@ -9669,7 +9865,7 @@
         <v>10</v>
       </c>
       <c r="C126" s="40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D126" s="5">
         <v>2</v>
@@ -9701,7 +9897,7 @@
         <v>9</v>
       </c>
       <c r="C127" s="40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D127" s="5">
         <v>2.09</v>
@@ -9733,7 +9929,7 @@
         <v>10</v>
       </c>
       <c r="C128" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D128" s="5">
         <v>1.95</v>
@@ -9765,7 +9961,7 @@
         <v>9</v>
       </c>
       <c r="C129" s="40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D129" s="5">
         <v>2.0299999999999998</v>
@@ -9829,7 +10025,7 @@
         <v>9</v>
       </c>
       <c r="C131" s="40" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D131" s="5">
         <v>1.99</v>
@@ -9861,7 +10057,7 @@
         <v>9</v>
       </c>
       <c r="C132" s="40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D132" s="5">
         <v>1.88</v>
@@ -9893,7 +10089,7 @@
         <v>9</v>
       </c>
       <c r="C133" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D133" s="5">
         <v>1.92</v>
@@ -9925,7 +10121,7 @@
         <v>9</v>
       </c>
       <c r="C134" s="40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D134" s="5">
         <v>1.79</v>
@@ -9957,7 +10153,7 @@
         <v>9</v>
       </c>
       <c r="C135" s="40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D135" s="5">
         <v>2.14</v>
@@ -10021,7 +10217,7 @@
         <v>10</v>
       </c>
       <c r="C137" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D137" s="5">
         <v>2.1</v>
@@ -10053,7 +10249,7 @@
         <v>10</v>
       </c>
       <c r="C138" s="83" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D138" s="56">
         <v>1.65</v>
@@ -10089,7 +10285,7 @@
         <v>10</v>
       </c>
       <c r="C139" s="40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D139" s="5">
         <v>1.83</v>
@@ -10121,7 +10317,7 @@
         <v>10</v>
       </c>
       <c r="C140" s="40" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D140" s="5">
         <v>1.91</v>
@@ -10153,7 +10349,7 @@
         <v>9</v>
       </c>
       <c r="C141" s="40" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D141" s="5">
         <v>2.44</v>
@@ -10185,7 +10381,7 @@
         <v>9</v>
       </c>
       <c r="C142" s="40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D142" s="5">
         <v>2.62</v>
@@ -10217,7 +10413,7 @@
         <v>9</v>
       </c>
       <c r="C143" s="40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D143" s="5">
         <v>1.81</v>
@@ -10249,7 +10445,7 @@
         <v>9</v>
       </c>
       <c r="C144" s="40" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D144" s="5">
         <v>1.9</v>
@@ -10313,7 +10509,7 @@
         <v>9</v>
       </c>
       <c r="C146" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D146" s="5">
         <v>1.99</v>
@@ -10345,7 +10541,7 @@
         <v>10</v>
       </c>
       <c r="C147" s="40" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D147" s="5">
         <v>1.87</v>
@@ -10377,7 +10573,7 @@
         <v>10</v>
       </c>
       <c r="C148" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D148" s="5">
         <v>2</v>
@@ -10409,7 +10605,7 @@
         <v>10</v>
       </c>
       <c r="C149" s="40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D149" s="5">
         <v>1.83</v>
@@ -10441,7 +10637,7 @@
         <v>9</v>
       </c>
       <c r="C150" s="40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D150" s="5">
         <v>1.93</v>
@@ -10473,7 +10669,7 @@
         <v>10</v>
       </c>
       <c r="C151" s="40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D151" s="5">
         <v>2.15</v>
@@ -10537,7 +10733,7 @@
         <v>9</v>
       </c>
       <c r="C153" s="40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D153" s="5">
         <v>1.78</v>
@@ -10601,7 +10797,7 @@
         <v>9</v>
       </c>
       <c r="C155" s="40" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D155" s="5">
         <v>1.75</v>
@@ -10633,7 +10829,7 @@
         <v>9</v>
       </c>
       <c r="C156" s="40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D156" s="5">
         <v>2.1</v>
@@ -10665,7 +10861,7 @@
         <v>9</v>
       </c>
       <c r="C157" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D157" s="5">
         <v>1.7</v>
@@ -10697,7 +10893,7 @@
         <v>9</v>
       </c>
       <c r="C158" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D158" s="5">
         <v>1.98</v>
@@ -10729,7 +10925,7 @@
         <v>9</v>
       </c>
       <c r="C159" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D159" s="5">
         <v>1.87</v>
@@ -10761,7 +10957,7 @@
         <v>9</v>
       </c>
       <c r="C160" s="40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D160" s="5">
         <v>1.62</v>
@@ -10793,7 +10989,7 @@
         <v>9</v>
       </c>
       <c r="C161" s="40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D161" s="5">
         <v>1.94</v>
@@ -10825,7 +11021,7 @@
         <v>9</v>
       </c>
       <c r="C162" s="40" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D162" s="5">
         <v>1.91</v>
@@ -10857,7 +11053,7 @@
         <v>9</v>
       </c>
       <c r="C163" s="40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D163" s="5">
         <v>1.76</v>
@@ -10889,7 +11085,7 @@
         <v>9</v>
       </c>
       <c r="C164" s="40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D164" s="5">
         <v>2.0099999999999998</v>
@@ -10921,7 +11117,7 @@
         <v>9</v>
       </c>
       <c r="C165" s="40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D165" s="5">
         <v>2.19</v>
@@ -10953,7 +11149,7 @@
         <v>9</v>
       </c>
       <c r="C166" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D166" s="5">
         <v>2.06</v>
@@ -10985,7 +11181,7 @@
         <v>9</v>
       </c>
       <c r="C167" s="40" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D167" s="5">
         <v>2.09</v>
@@ -11017,7 +11213,7 @@
         <v>9</v>
       </c>
       <c r="C168" s="40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D168" s="5">
         <v>2.14</v>
@@ -11049,7 +11245,7 @@
         <v>9</v>
       </c>
       <c r="C169" s="40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D169" s="5">
         <v>1.74</v>
@@ -11149,7 +11345,7 @@
         <v>9</v>
       </c>
       <c r="C172" s="40" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D172" s="5">
         <v>1.97</v>
@@ -11181,7 +11377,7 @@
         <v>9</v>
       </c>
       <c r="C173" s="40" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D173" s="5">
         <v>2.17</v>
@@ -11213,7 +11409,7 @@
         <v>9</v>
       </c>
       <c r="C174" s="40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D174" s="5">
         <v>2.04</v>
@@ -11245,7 +11441,7 @@
         <v>9</v>
       </c>
       <c r="C175" s="40" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D175" s="5">
         <v>1.99</v>
@@ -11309,7 +11505,7 @@
         <v>9</v>
       </c>
       <c r="C177" s="40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D177" s="5">
         <v>1.98</v>
@@ -11341,7 +11537,7 @@
         <v>9</v>
       </c>
       <c r="C178" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D178" s="5">
         <v>1.91</v>
@@ -11373,7 +11569,7 @@
         <v>9</v>
       </c>
       <c r="C179" s="40" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D179" s="5">
         <v>1.95</v>
@@ -11405,7 +11601,7 @@
         <v>9</v>
       </c>
       <c r="C180" s="40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D180" s="5">
         <v>1.89</v>
@@ -11437,7 +11633,7 @@
         <v>9</v>
       </c>
       <c r="C181" s="40" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D181" s="5">
         <v>1.76</v>
@@ -11469,7 +11665,7 @@
         <v>9</v>
       </c>
       <c r="C182" s="40" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D182" s="5">
         <v>2</v>
@@ -11501,7 +11697,7 @@
         <v>9</v>
       </c>
       <c r="C183" s="40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D183" s="5">
         <v>1.74</v>
@@ -11533,7 +11729,7 @@
         <v>10</v>
       </c>
       <c r="C184" s="83" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D184" s="56">
         <v>2</v>
@@ -11569,7 +11765,7 @@
         <v>9</v>
       </c>
       <c r="C185" s="40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D185" s="5">
         <v>2.0699999999999998</v>
@@ -11581,15 +11777,15 @@
         <v>15</v>
       </c>
       <c r="J185" s="69">
-        <f t="shared" ref="J185:J214" si="29">IF(I185="", 0, IF(I185="Win", F185*D185-F185, -F185))</f>
+        <f t="shared" ref="J185:J217" si="29">IF(I185="", 0, IF(I185="Win", F185*D185-F185, -F185))</f>
         <v>10.7</v>
       </c>
       <c r="L185" s="45">
-        <f t="shared" ref="L185:L214" si="30">ROUND(-K185*J185, 2)</f>
+        <f t="shared" ref="L185:L217" si="30">ROUND(-K185*J185, 2)</f>
         <v>0</v>
       </c>
       <c r="M185" s="46">
-        <f t="shared" ref="M185:M214" si="31">J185+L185</f>
+        <f t="shared" ref="M185:M217" si="31">J185+L185</f>
         <v>10.7</v>
       </c>
     </row>
@@ -11600,8 +11796,8 @@
       <c r="B186" t="s">
         <v>9</v>
       </c>
-      <c r="C186" s="94" t="s">
-        <v>214</v>
+      <c r="C186" s="93" t="s">
+        <v>212</v>
       </c>
       <c r="D186" s="5">
         <v>1.91</v>
@@ -11632,8 +11828,8 @@
       <c r="B187" t="s">
         <v>9</v>
       </c>
-      <c r="C187" s="94" t="s">
-        <v>216</v>
+      <c r="C187" s="93" t="s">
+        <v>214</v>
       </c>
       <c r="D187" s="5">
         <v>1.95</v>
@@ -11665,7 +11861,7 @@
         <v>9</v>
       </c>
       <c r="C188" s="40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D188" s="5">
         <v>1.96</v>
@@ -11697,7 +11893,7 @@
         <v>9</v>
       </c>
       <c r="C189" s="40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D189" s="5">
         <v>1.76</v>
@@ -11729,7 +11925,7 @@
         <v>9</v>
       </c>
       <c r="C190" s="40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D190" s="5">
         <v>1.92</v>
@@ -11761,7 +11957,7 @@
         <v>9</v>
       </c>
       <c r="C191" s="40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D191" s="5">
         <v>2.13</v>
@@ -11793,7 +11989,7 @@
         <v>9</v>
       </c>
       <c r="C192" s="40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D192" s="5">
         <v>1.7</v>
@@ -11857,7 +12053,7 @@
         <v>9</v>
       </c>
       <c r="C194" s="40" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D194" s="5">
         <v>1.74</v>
@@ -11921,7 +12117,7 @@
         <v>9</v>
       </c>
       <c r="C196" s="40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D196" s="5">
         <v>2.25</v>
@@ -11953,7 +12149,7 @@
         <v>10</v>
       </c>
       <c r="C197" s="40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D197" s="5">
         <v>1.87</v>
@@ -11985,7 +12181,7 @@
         <v>9</v>
       </c>
       <c r="C198" s="40" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D198" s="5">
         <v>2.04</v>
@@ -12017,7 +12213,7 @@
         <v>9</v>
       </c>
       <c r="C199" s="40" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D199" s="5">
         <v>1.88</v>
@@ -12049,7 +12245,7 @@
         <v>9</v>
       </c>
       <c r="C200" s="40" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D200" s="5">
         <v>2.1</v>
@@ -12081,7 +12277,7 @@
         <v>9</v>
       </c>
       <c r="C201" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D201" s="5">
         <v>1.55</v>
@@ -12113,7 +12309,7 @@
         <v>9</v>
       </c>
       <c r="C202" s="40" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D202" s="5">
         <v>1.87</v>
@@ -12145,7 +12341,7 @@
         <v>9</v>
       </c>
       <c r="C203" s="40" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D203" s="5">
         <v>1.87</v>
@@ -12177,7 +12373,7 @@
         <v>10</v>
       </c>
       <c r="C204" s="40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D204" s="5">
         <v>1.83</v>
@@ -12209,7 +12405,7 @@
         <v>10</v>
       </c>
       <c r="C205" s="83" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D205" s="56">
         <v>1.87</v>
@@ -12245,7 +12441,7 @@
         <v>9</v>
       </c>
       <c r="C206" s="40" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D206" s="5">
         <v>2.0099999999999998</v>
@@ -12277,7 +12473,7 @@
         <v>9</v>
       </c>
       <c r="C207" s="40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D207" s="5">
         <v>1.61</v>
@@ -12341,7 +12537,7 @@
         <v>9</v>
       </c>
       <c r="C209" s="40" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D209" s="5">
         <v>1.79</v>
@@ -12350,7 +12546,7 @@
         <v>10</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J209" s="69">
         <f t="shared" si="29"/>
@@ -12373,7 +12569,7 @@
         <v>9</v>
       </c>
       <c r="C210" s="40" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D210" s="5">
         <v>2</v>
@@ -12382,7 +12578,7 @@
         <v>10</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J210" s="69">
         <f t="shared" si="29"/>
@@ -12405,7 +12601,7 @@
         <v>10</v>
       </c>
       <c r="C211" s="43" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D211" s="7">
         <v>1.78</v>
@@ -12441,7 +12637,7 @@
         <v>10</v>
       </c>
       <c r="C212" s="40" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D212" s="5">
         <v>1.87</v>
@@ -12473,7 +12669,7 @@
         <v>10</v>
       </c>
       <c r="C213" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D213" s="5">
         <v>2.1</v>
@@ -12505,7 +12701,7 @@
         <v>10</v>
       </c>
       <c r="C214" s="83" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D214" s="56">
         <v>1.83</v>
@@ -12531,6 +12727,106 @@
       <c r="M214" s="72">
         <f t="shared" si="31"/>
         <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A215" s="34">
+        <v>43481</v>
+      </c>
+      <c r="B215" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C215" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="D215" s="5">
+        <v>2</v>
+      </c>
+      <c r="F215" s="6">
+        <v>10</v>
+      </c>
+      <c r="I215" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J215" s="69">
+        <f t="shared" si="29"/>
+        <v>10</v>
+      </c>
+      <c r="L215" s="45">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="M215" s="46">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A216" s="34">
+        <v>43481</v>
+      </c>
+      <c r="B216" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D216" s="5">
+        <v>1.83</v>
+      </c>
+      <c r="F216" s="6">
+        <v>10</v>
+      </c>
+      <c r="I216" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J216" s="69">
+        <f t="shared" si="29"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L216" s="45">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="M216" s="46">
+        <f t="shared" si="31"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="37">
+        <v>43481</v>
+      </c>
+      <c r="B217" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C217" s="83" t="s">
+        <v>238</v>
+      </c>
+      <c r="D217" s="56">
+        <v>2.15</v>
+      </c>
+      <c r="E217" s="56"/>
+      <c r="F217" s="38">
+        <v>10</v>
+      </c>
+      <c r="G217" s="63"/>
+      <c r="H217" s="64"/>
+      <c r="I217" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="J217" s="51">
+        <f t="shared" si="29"/>
+        <v>11.5</v>
+      </c>
+      <c r="K217" s="39"/>
+      <c r="L217" s="20">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="M217" s="72">
+        <f t="shared" si="31"/>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>
@@ -12576,7 +12872,7 @@
       <formula>"Betfair"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C172:C185 C188:C214">
+  <conditionalFormatting sqref="C172:C185 C188:C217">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Ladbrokes"</formula>
     </cfRule>
@@ -12649,7 +12945,7 @@
         <v>102</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
@@ -12698,11 +12994,11 @@
       </c>
       <c r="D4" s="78">
         <f>SUMIFS(Master!F:F,Master!B:B,Exchange!B4)</f>
-        <v>1753.8</v>
+        <v>1773.8</v>
       </c>
       <c r="E4" s="80">
         <f>COUNTIF(Master!B:B,Exchange!B4)</f>
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F4" s="45">
         <f t="shared" si="0"/>
@@ -12710,11 +13006,11 @@
       </c>
       <c r="G4" s="78">
         <f>SUMIFS(Master!M:M, Master!B:B,Exchange!B4)</f>
-        <v>-283.63000000000005</v>
+        <v>-265.33000000000004</v>
       </c>
       <c r="H4" s="78">
         <f t="shared" si="1"/>
-        <v>241.36999999999995</v>
+        <v>259.66999999999996</v>
       </c>
       <c r="J4" s="75">
         <v>43456</v>
@@ -12735,11 +13031,11 @@
       </c>
       <c r="D5" s="78">
         <f>SUMIFS(Master!F:F,Master!B:B,Exchange!B5)</f>
-        <v>1024.8</v>
+        <v>1034.8</v>
       </c>
       <c r="E5" s="80">
         <f>COUNTIF(Master!B:B,Exchange!B5)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F5" s="45">
         <f t="shared" si="0"/>
@@ -12747,11 +13043,11 @@
       </c>
       <c r="G5" s="78">
         <f>SUMIFS(Master!M:M, Master!B:B,Exchange!B5)</f>
-        <v>226.73000000000008</v>
+        <v>238.23000000000008</v>
       </c>
       <c r="H5" s="78">
         <f t="shared" ref="H5:H6" si="2">SUM(C5,F5,G5)</f>
-        <v>310.93000000000006</v>
+        <v>322.43000000000006</v>
       </c>
       <c r="J5" s="75">
         <v>43461</v>
@@ -12779,11 +13075,11 @@
       </c>
       <c r="G6" s="79">
         <f t="shared" si="3"/>
-        <v>74.850000000000023</v>
+        <v>104.65000000000003</v>
       </c>
       <c r="H6" s="79">
         <f t="shared" si="2"/>
-        <v>652.76</v>
+        <v>682.56</v>
       </c>
       <c r="J6" s="75">
         <v>43462</v>

</xml_diff>